<commit_message>
Regretion Run SCD0177 - SCD0186
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0177_Validasi BNIMF.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0177_Validasi BNIMF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE23DAC-DB64-47D5-BFF5-1C9A3E883203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C599317-EE15-499A-AB3A-E9BA354CFA6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1680" yWindow="3630" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCD0177" sheetId="2" r:id="rId1"/>
@@ -164,7 +164,7 @@
     <t>Bukti bahwa npp 49998 tidak memiliki kode outlet</t>
   </si>
   <si>
-    <t>Leads Prospek NULL 09</t>
+    <t>Leads Prospek NULL 10</t>
   </si>
 </sst>
 </file>

</xml_diff>